<commit_message>
增加各种寄存器类型支持，apb, axi, ocp, wishbone, user define
</commit_message>
<xml_diff>
--- a/autoregfile/examples/configs/example_config.xlsx
+++ b/autoregfile/examples/configs/example_config.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,52 +482,64 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>num_write_ports</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
+          <t>bus_protocol</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>apb</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>num_read_ports</t>
+          <t>num_write_ports</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sync_reset</t>
-        </is>
-      </c>
-      <c r="B7" t="b">
-        <v>0</v>
+          <t>num_read_ports</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>reset_value</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0x00000000</t>
-        </is>
+          <t>sync_reset</t>
+        </is>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>reset_value</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0x00000000</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>byte_enable</t>
         </is>
       </c>
-      <c r="B9" t="b">
+      <c r="B10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -644,7 +656,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ReadClean</t>
+          <t>Write1Clear</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>